<commit_message>
read from excel method
</commit_message>
<xml_diff>
--- a/exercises/exercise_1/data/riket2023_åk9_np.xlsx
+++ b/exercises/exercise_1/data/riket2023_åk9_np.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="Engelska"/>
@@ -144,7 +144,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -161,7 +161,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -177,12 +177,6 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -213,7 +207,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -241,12 +235,6 @@
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -638,7 +626,7 @@
   </sheetPr>
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView workbookViewId="0" tabSelected="1">
       <pane state="frozen" activePane="bottomLeft" topLeftCell="A10" ySplit="9" xSplit="0"/>
     </sheetView>
   </sheetViews>
@@ -646,15 +634,15 @@
   <cols>
     <col min="1" max="1" style="3" width="10.005" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="3" width="14.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="12" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="12" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="12" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="13" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="13" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="13" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="13" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="13" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="13" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="10" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="10" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="10" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="11" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="11" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="11" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="11" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="11" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="11" width="12.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
@@ -815,31 +803,31 @@
       <c r="B10" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10" s="4">
         <v>106941</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="4">
         <v>51864</v>
       </c>
-      <c r="E10" s="10">
+      <c r="E10" s="4">
         <v>55077</v>
       </c>
-      <c r="F10" s="11">
+      <c r="F10" s="5">
         <v>97</v>
       </c>
-      <c r="G10" s="11">
+      <c r="G10" s="5">
         <v>97.1</v>
       </c>
-      <c r="H10" s="11">
+      <c r="H10" s="5">
         <v>97</v>
       </c>
-      <c r="I10" s="11">
+      <c r="I10" s="5">
         <v>15.7</v>
       </c>
-      <c r="J10" s="11">
+      <c r="J10" s="5">
         <v>15.8</v>
       </c>
-      <c r="K10" s="11">
+      <c r="K10" s="5">
         <v>15.7</v>
       </c>
     </row>
@@ -850,31 +838,31 @@
       <c r="B11" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C11" s="4">
         <v>84310</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D11" s="4">
         <v>40675</v>
       </c>
-      <c r="E11" s="10">
+      <c r="E11" s="4">
         <v>43635</v>
       </c>
-      <c r="F11" s="11">
+      <c r="F11" s="5">
         <v>96.6</v>
       </c>
-      <c r="G11" s="11">
+      <c r="G11" s="5">
         <v>96.6</v>
       </c>
-      <c r="H11" s="11">
+      <c r="H11" s="5">
         <v>96.6</v>
       </c>
-      <c r="I11" s="11">
+      <c r="I11" s="5">
         <v>15.4</v>
       </c>
-      <c r="J11" s="11">
+      <c r="J11" s="5">
         <v>15.5</v>
       </c>
-      <c r="K11" s="11">
+      <c r="K11" s="5">
         <v>15.4</v>
       </c>
     </row>
@@ -885,31 +873,31 @@
       <c r="B12" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="10">
+      <c r="C12" s="4">
         <v>22582</v>
       </c>
-      <c r="D12" s="10">
+      <c r="D12" s="4">
         <v>11165</v>
       </c>
-      <c r="E12" s="10">
+      <c r="E12" s="4">
         <v>11417</v>
       </c>
-      <c r="F12" s="11">
+      <c r="F12" s="5">
         <v>98.7</v>
       </c>
-      <c r="G12" s="11">
+      <c r="G12" s="5">
         <v>98.8</v>
       </c>
-      <c r="H12" s="11">
+      <c r="H12" s="5">
         <v>98.7</v>
       </c>
-      <c r="I12" s="11">
+      <c r="I12" s="5">
         <v>16.9</v>
       </c>
-      <c r="J12" s="11">
+      <c r="J12" s="5">
         <v>17</v>
       </c>
-      <c r="K12" s="11">
+      <c r="K12" s="5">
         <v>16.8</v>
       </c>
     </row>
@@ -920,31 +908,31 @@
       <c r="B13" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="10">
+      <c r="C13" s="4">
         <v>49</v>
       </c>
-      <c r="D13" s="10">
+      <c r="D13" s="4">
         <v>24</v>
       </c>
-      <c r="E13" s="10">
+      <c r="E13" s="4">
         <v>25</v>
       </c>
-      <c r="F13" s="11">
+      <c r="F13" s="5">
         <v>100</v>
       </c>
-      <c r="G13" s="11">
+      <c r="G13" s="5">
         <v>100</v>
       </c>
-      <c r="H13" s="11">
+      <c r="H13" s="5">
         <v>100</v>
       </c>
-      <c r="I13" s="11">
+      <c r="I13" s="5">
         <v>18.5</v>
       </c>
-      <c r="J13" s="11">
+      <c r="J13" s="5">
         <v>18.9</v>
       </c>
-      <c r="K13" s="11">
+      <c r="K13" s="5">
         <v>18.2</v>
       </c>
     </row>
@@ -968,7 +956,7 @@
   </sheetPr>
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1">
+    <sheetView workbookViewId="0">
       <pane state="frozen" activePane="bottomLeft" topLeftCell="A10" ySplit="9" xSplit="0"/>
     </sheetView>
   </sheetViews>
@@ -976,15 +964,15 @@
   <cols>
     <col min="1" max="1" style="3" width="10.005" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="3" width="14.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="12" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="12" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="12" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="13" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="13" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="13" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="13" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="13" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="13" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="10" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="10" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="10" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="11" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="11" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="11" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="11" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="11" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="11" width="12.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
@@ -1138,143 +1126,143 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="21.75">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10" s="4">
         <v>106766</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="4">
         <v>51548</v>
       </c>
-      <c r="E10" s="10">
+      <c r="E10" s="4">
         <v>55218</v>
       </c>
-      <c r="F10" s="11">
+      <c r="F10" s="5">
         <v>89.1</v>
       </c>
-      <c r="G10" s="11">
+      <c r="G10" s="5">
         <v>88.7</v>
       </c>
-      <c r="H10" s="11">
+      <c r="H10" s="5">
         <v>89.5</v>
       </c>
-      <c r="I10" s="11">
+      <c r="I10" s="5">
         <v>11.9</v>
       </c>
-      <c r="J10" s="11">
+      <c r="J10" s="5">
         <v>11.8</v>
       </c>
-      <c r="K10" s="11">
+      <c r="K10" s="5">
         <v>12</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="21.75">
       <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C11" s="4">
         <v>84163</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D11" s="4">
         <v>40386</v>
       </c>
-      <c r="E11" s="10">
+      <c r="E11" s="4">
         <v>43777</v>
       </c>
-      <c r="F11" s="11">
+      <c r="F11" s="5">
         <v>88.1</v>
       </c>
-      <c r="G11" s="11">
+      <c r="G11" s="5">
         <v>87.7</v>
       </c>
-      <c r="H11" s="11">
+      <c r="H11" s="5">
         <v>88.5</v>
       </c>
-      <c r="I11" s="11">
+      <c r="I11" s="5">
         <v>11.6</v>
       </c>
-      <c r="J11" s="11">
+      <c r="J11" s="5">
         <v>11.5</v>
       </c>
-      <c r="K11" s="11">
+      <c r="K11" s="5">
         <v>11.7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="21.75">
       <c r="A12" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="10">
+      <c r="C12" s="4">
         <v>22553</v>
       </c>
-      <c r="D12" s="10">
+      <c r="D12" s="4">
         <v>11137</v>
       </c>
-      <c r="E12" s="10">
+      <c r="E12" s="4">
         <v>11416</v>
       </c>
-      <c r="F12" s="11">
+      <c r="F12" s="5">
         <v>92.9</v>
       </c>
-      <c r="G12" s="11">
+      <c r="G12" s="5">
         <v>92.2</v>
       </c>
-      <c r="H12" s="11">
+      <c r="H12" s="5">
         <v>93.5</v>
       </c>
-      <c r="I12" s="11">
+      <c r="I12" s="5">
         <v>13</v>
       </c>
-      <c r="J12" s="11">
+      <c r="J12" s="5">
         <v>12.8</v>
       </c>
-      <c r="K12" s="11">
+      <c r="K12" s="5">
         <v>13.1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="21.75">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="10">
+      <c r="C13" s="4">
         <v>50</v>
       </c>
-      <c r="D13" s="10">
+      <c r="D13" s="4">
         <v>25</v>
       </c>
-      <c r="E13" s="10">
+      <c r="E13" s="4">
         <v>25</v>
       </c>
-      <c r="F13" s="11" t="s">
+      <c r="F13" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="G13" s="11" t="s">
+      <c r="G13" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="H13" s="11" t="s">
+      <c r="H13" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="I13" s="11">
+      <c r="I13" s="5">
         <v>14.1</v>
       </c>
-      <c r="J13" s="11">
+      <c r="J13" s="5">
         <v>13.5</v>
       </c>
-      <c r="K13" s="11">
+      <c r="K13" s="5">
         <v>14.7</v>
       </c>
     </row>
@@ -1306,15 +1294,15 @@
   <cols>
     <col min="1" max="1" style="3" width="10.005" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="3" width="14.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="12" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="12" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="12" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="13" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="13" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="13" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="13" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="13" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="13" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="10" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="10" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="10" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="11" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="11" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="11" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="11" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="11" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="11" width="12.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
@@ -1475,31 +1463,31 @@
       <c r="B10" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10" s="4">
         <v>93225</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="4">
         <v>45800</v>
       </c>
-      <c r="E10" s="10">
+      <c r="E10" s="4">
         <v>47425</v>
       </c>
-      <c r="F10" s="11">
+      <c r="F10" s="5">
         <v>96.1</v>
       </c>
-      <c r="G10" s="11">
+      <c r="G10" s="5">
         <v>97.9</v>
       </c>
-      <c r="H10" s="11">
+      <c r="H10" s="5">
         <v>94.4</v>
       </c>
-      <c r="I10" s="11">
+      <c r="I10" s="5">
         <v>13.6</v>
       </c>
-      <c r="J10" s="11">
+      <c r="J10" s="5">
         <v>14.5</v>
       </c>
-      <c r="K10" s="11">
+      <c r="K10" s="5">
         <v>12.7</v>
       </c>
     </row>
@@ -1510,31 +1498,31 @@
       <c r="B11" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C11" s="4">
         <v>72771</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D11" s="4">
         <v>35484</v>
       </c>
-      <c r="E11" s="10">
+      <c r="E11" s="4">
         <v>37287</v>
       </c>
-      <c r="F11" s="11">
+      <c r="F11" s="5">
         <v>95.7</v>
       </c>
-      <c r="G11" s="11">
+      <c r="G11" s="5">
         <v>97.6</v>
       </c>
-      <c r="H11" s="11">
+      <c r="H11" s="5">
         <v>93.8</v>
       </c>
-      <c r="I11" s="11">
+      <c r="I11" s="5">
         <v>13.3</v>
       </c>
-      <c r="J11" s="11">
+      <c r="J11" s="5">
         <v>14.3</v>
       </c>
-      <c r="K11" s="11">
+      <c r="K11" s="5">
         <v>12.4</v>
       </c>
     </row>
@@ -1545,31 +1533,31 @@
       <c r="B12" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="10">
+      <c r="C12" s="4">
         <v>20414</v>
       </c>
-      <c r="D12" s="10">
+      <c r="D12" s="4">
         <v>10297</v>
       </c>
-      <c r="E12" s="10">
+      <c r="E12" s="4">
         <v>10117</v>
       </c>
-      <c r="F12" s="11">
+      <c r="F12" s="5">
         <v>97.6</v>
       </c>
-      <c r="G12" s="11">
+      <c r="G12" s="5">
         <v>98.7</v>
       </c>
-      <c r="H12" s="11">
+      <c r="H12" s="5">
         <v>96.6</v>
       </c>
-      <c r="I12" s="11">
+      <c r="I12" s="5">
         <v>14.4</v>
       </c>
-      <c r="J12" s="11">
+      <c r="J12" s="5">
         <v>15.2</v>
       </c>
-      <c r="K12" s="11">
+      <c r="K12" s="5">
         <v>13.5</v>
       </c>
     </row>
@@ -1580,31 +1568,31 @@
       <c r="B13" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="10">
+      <c r="C13" s="4">
         <v>40</v>
       </c>
-      <c r="D13" s="10">
+      <c r="D13" s="4">
         <v>19</v>
       </c>
-      <c r="E13" s="10">
+      <c r="E13" s="4">
         <v>21</v>
       </c>
-      <c r="F13" s="11">
+      <c r="F13" s="5">
         <v>100</v>
       </c>
-      <c r="G13" s="11">
+      <c r="G13" s="5">
         <v>100</v>
       </c>
-      <c r="H13" s="11">
+      <c r="H13" s="5">
         <v>100</v>
       </c>
-      <c r="I13" s="11">
+      <c r="I13" s="5">
         <v>15</v>
       </c>
-      <c r="J13" s="11">
+      <c r="J13" s="5">
         <v>15.9</v>
       </c>
-      <c r="K13" s="11">
+      <c r="K13" s="5">
         <v>14.2</v>
       </c>
     </row>
@@ -1636,15 +1624,15 @@
   <cols>
     <col min="1" max="1" style="3" width="10.005" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="3" width="14.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="12" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="12" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="12" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="13" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="13" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="13" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="13" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="13" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="13" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="10" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="10" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="10" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="11" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="11" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="11" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="11" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="11" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="11" width="12.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
@@ -1805,31 +1793,31 @@
       <c r="B10" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10" s="4">
         <v>14092</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="4">
         <v>6447</v>
       </c>
-      <c r="E10" s="10">
+      <c r="E10" s="4">
         <v>7645</v>
       </c>
-      <c r="F10" s="11">
+      <c r="F10" s="5">
         <v>77.7</v>
       </c>
-      <c r="G10" s="11">
+      <c r="G10" s="5">
         <v>81.6</v>
       </c>
-      <c r="H10" s="11">
+      <c r="H10" s="5">
         <v>74.3</v>
       </c>
-      <c r="I10" s="11">
+      <c r="I10" s="5">
         <v>9.4</v>
       </c>
-      <c r="J10" s="11">
+      <c r="J10" s="5">
         <v>10.2</v>
       </c>
-      <c r="K10" s="11">
+      <c r="K10" s="5">
         <v>8.7</v>
       </c>
     </row>
@@ -1840,31 +1828,31 @@
       <c r="B11" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C11" s="4">
         <v>11963</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D11" s="4">
         <v>5495</v>
       </c>
-      <c r="E11" s="10">
+      <c r="E11" s="4">
         <v>6468</v>
       </c>
-      <c r="F11" s="11">
+      <c r="F11" s="5">
         <v>75.9</v>
       </c>
-      <c r="G11" s="11">
+      <c r="G11" s="5">
         <v>80</v>
       </c>
-      <c r="H11" s="11">
+      <c r="H11" s="5">
         <v>72.4</v>
       </c>
-      <c r="I11" s="11">
+      <c r="I11" s="5">
         <v>9</v>
       </c>
-      <c r="J11" s="11">
+      <c r="J11" s="5">
         <v>9.9</v>
       </c>
-      <c r="K11" s="11">
+      <c r="K11" s="5">
         <v>8.3</v>
       </c>
     </row>
@@ -1875,31 +1863,31 @@
       <c r="B12" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="10">
+      <c r="C12" s="4">
         <v>2122</v>
       </c>
-      <c r="D12" s="10">
+      <c r="D12" s="4">
         <v>949</v>
       </c>
-      <c r="E12" s="10">
+      <c r="E12" s="4">
         <v>1173</v>
       </c>
-      <c r="F12" s="11">
+      <c r="F12" s="5">
         <v>87.7</v>
       </c>
-      <c r="G12" s="11">
+      <c r="G12" s="5">
         <v>90.9</v>
       </c>
-      <c r="H12" s="11">
+      <c r="H12" s="5">
         <v>85.2</v>
       </c>
-      <c r="I12" s="11">
+      <c r="I12" s="5">
         <v>11.1</v>
       </c>
-      <c r="J12" s="11">
+      <c r="J12" s="5">
         <v>12</v>
       </c>
-      <c r="K12" s="11">
+      <c r="K12" s="5">
         <v>10.4</v>
       </c>
     </row>
@@ -1910,31 +1898,31 @@
       <c r="B13" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E13" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="F13" s="11" t="s">
+      <c r="F13" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="G13" s="11" t="s">
+      <c r="G13" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="H13" s="11" t="s">
+      <c r="H13" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="I13" s="11" t="s">
+      <c r="I13" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="J13" s="11" t="s">
+      <c r="J13" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="K13" s="11" t="s">
+      <c r="K13" s="5" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>